<commit_message>
updated loadbase to ignore errors
</commit_message>
<xml_diff>
--- a/data/Excel Format/entities/Student.xlsx
+++ b/data/Excel Format/entities/Student.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="336">
   <si>
     <t>id</t>
   </si>
@@ -39,6 +39,12 @@
     <t>description</t>
   </si>
   <si>
+    <t>semester</t>
+  </si>
+  <si>
+    <t>year_in</t>
+  </si>
+  <si>
     <t>milsmith@uwaterloo.ca</t>
   </si>
   <si>
@@ -57,6 +63,9 @@
     <t>Todo</t>
   </si>
   <si>
+    <t>Fall</t>
+  </si>
+  <si>
     <t>chrjohns@uwaterloo.ca</t>
   </si>
   <si>
@@ -66,6 +75,9 @@
     <t>Johnson</t>
   </si>
   <si>
+    <t>Winter</t>
+  </si>
+  <si>
     <t>jeawilli@uwaterloo.ca</t>
   </si>
   <si>
@@ -91,6 +103,9 @@
   </si>
   <si>
     <t>2A</t>
+  </si>
+  <si>
+    <t>Spring</t>
   </si>
   <si>
     <t>asybrown@uwaterloo.ca</t>
@@ -1015,7 +1030,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -1031,6 +1046,11 @@
       <u/>
       <sz val="11.0"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -1081,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1090,14 +1110,20 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1348,28 +1374,40 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
         <v>9.6667175E7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="3">
@@ -1377,22 +1415,28 @@
         <v>7.356463E7</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="4">
@@ -1400,22 +1444,28 @@
         <v>5.1458338E7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
+      <c r="I4" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="5">
@@ -1423,22 +1473,28 @@
         <v>4.5453885E7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="6">
@@ -1446,22 +1502,28 @@
         <v>7.9689206E7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
+      <c r="I6" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="7">
@@ -1469,22 +1531,28 @@
         <v>6.7496942E7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="8">
@@ -1492,22 +1560,28 @@
         <v>4.0128931E7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="9">
@@ -1515,22 +1589,28 @@
         <v>1.976751E7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="10">
@@ -1538,22 +1618,28 @@
         <v>8.3950021E7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="11">
@@ -1561,22 +1647,28 @@
         <v>9.126056E7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="12">
@@ -1584,22 +1676,28 @@
         <v>6.0653931E7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="13">
@@ -1607,22 +1705,28 @@
         <v>2.2779613E7</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="14">
@@ -1630,2000 +1734,2522 @@
         <v>1.3336678E7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
         <v>2.1217676E7</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>59</v>
+      <c r="B15" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
         <v>3.4566543E7</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>63</v>
+      <c r="B16" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
         <v>3.7486905E7</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>68</v>
+      <c r="B17" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
         <v>9.2514073E7</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>72</v>
+      <c r="B18" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
         <v>1.0871349E7</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>75</v>
+      <c r="B19" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
         <v>6.2389417E7</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>79</v>
+      <c r="B20" s="6" t="s">
+        <v>84</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1">
         <v>2.9586401E7</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>82</v>
+      <c r="B21" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>86</v>
+      <c r="I21" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1">
         <v>5.4173986E7</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>87</v>
+      <c r="B22" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>91</v>
+      <c r="I22" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1">
         <v>7.5628493E7</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>92</v>
+      <c r="B23" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1">
         <v>2.3849065E7</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>96</v>
+      <c r="B24" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1">
         <v>9.6017348E7</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>100</v>
+      <c r="B25" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1">
         <v>1.8235964E7</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>104</v>
+      <c r="B26" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1">
         <v>6.5971234E7</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>108</v>
+      <c r="B27" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I27" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1">
         <v>4.8326591E7</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>112</v>
+      <c r="B28" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1">
         <v>7.1420935E7</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>114</v>
+      <c r="B29" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I29" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1">
         <v>5.2613498E7</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>118</v>
+      <c r="B30" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="1">
         <v>3.9827615E7</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>122</v>
+      <c r="B31" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I31" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1">
         <v>4.333499E7</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>125</v>
+      <c r="B32" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>128</v>
+        <v>133</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1">
         <v>2.8349567E7</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>129</v>
+      <c r="B33" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I33" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1">
         <v>9.1827364E7</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>132</v>
+      <c r="B34" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1">
         <v>7.2819365E7</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>135</v>
+      <c r="B35" s="7" t="s">
+        <v>140</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I35" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="1">
         <v>3.7482931E7</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>139</v>
+      <c r="B36" s="7" t="s">
+        <v>144</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>142</v>
+        <v>147</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="1">
         <v>9.3746281E7</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>143</v>
+      <c r="B37" s="7" t="s">
+        <v>148</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>146</v>
+        <v>151</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I37" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="1">
         <v>6.4927183E7</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>147</v>
+      <c r="B38" s="7" t="s">
+        <v>152</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>149</v>
+        <v>28</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="1">
         <v>1.837294E7</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>150</v>
+      <c r="B39" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="1">
         <v>5.2468719E7</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>154</v>
+      <c r="B40" s="7" t="s">
+        <v>159</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>156</v>
+        <v>161</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="1">
         <v>2.837491E7</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>157</v>
+      <c r="B41" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>158</v>
+        <v>163</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I41" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="1">
         <v>1.8472039E7</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>159</v>
+      <c r="B42" s="7" t="s">
+        <v>164</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I42" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="1">
         <v>8.5719236E7</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>161</v>
+      <c r="B43" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1">
         <v>4.9283617E7</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>162</v>
+      <c r="B44" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I44" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="1">
         <v>2.837461E7</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>165</v>
+      <c r="B45" s="7" t="s">
+        <v>170</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>167</v>
+        <v>172</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I45" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="1">
         <v>1.0293847E7</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>168</v>
+      <c r="B46" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>149</v>
+        <v>154</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I46" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="1">
         <v>3.7492816E7</v>
       </c>
-      <c r="B47" s="5" t="s">
-        <v>171</v>
+      <c r="B47" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>138</v>
+        <v>143</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="1">
         <v>8.5927361E7</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>172</v>
+      <c r="B48" s="7" t="s">
+        <v>177</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>173</v>
+        <v>178</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I48" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="1">
         <v>1.6273849E7</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>174</v>
+      <c r="B49" s="7" t="s">
+        <v>179</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>175</v>
+        <v>180</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I49" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="1">
         <v>3.9485671E7</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>176</v>
+      <c r="B50" s="7" t="s">
+        <v>181</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>177</v>
+        <v>182</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I50" s="5">
+        <v>2020.0</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="1">
         <v>6.2738495E7</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>178</v>
+      <c r="B51" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I51" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="1">
         <v>8.5719263E7</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>180</v>
+      <c r="B52" s="7" t="s">
+        <v>185</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="1">
         <v>2.9384756E7</v>
       </c>
-      <c r="B53" s="5" t="s">
-        <v>182</v>
+      <c r="B53" s="7" t="s">
+        <v>187</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H53" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F53" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>183</v>
+      <c r="I53" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="1">
         <v>1.7482936E7</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>184</v>
+      <c r="B54" s="7" t="s">
+        <v>189</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>185</v>
+        <v>190</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I54" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="1">
         <v>8.2917364E7</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>186</v>
+      <c r="B55" s="7" t="s">
+        <v>191</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>187</v>
+        <v>192</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I55" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="1">
         <v>2.7384916E7</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>188</v>
+      <c r="B56" s="7" t="s">
+        <v>193</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>189</v>
+        <v>194</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I56" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="1">
         <v>3.8491725E7</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>190</v>
+      <c r="B57" s="7" t="s">
+        <v>195</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E57" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H57" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F57" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>191</v>
+      <c r="I57" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1">
         <v>7.2918346E7</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>192</v>
+      <c r="B58" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>193</v>
+        <v>198</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I58" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="1">
         <v>2.9384617E7</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>194</v>
+      <c r="B59" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>195</v>
+        <v>200</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I59" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="1">
         <v>1.847392E7</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>196</v>
+      <c r="B60" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
+      </c>
+      <c r="H60" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I60" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="1">
         <v>4.9283651E7</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>198</v>
+      <c r="B61" s="7" t="s">
+        <v>203</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I61" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="1">
         <v>1.9384762E7</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>201</v>
+      <c r="B62" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I62" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="1">
         <v>1.2345678E7</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>203</v>
+      <c r="B63" s="7" t="s">
+        <v>208</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>204</v>
+        <v>209</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I63" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="1">
         <v>2.3456789E7</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>205</v>
+      <c r="B64" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>207</v>
+        <v>212</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I64" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="1">
         <v>3.456789E7</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>208</v>
+      <c r="B65" s="7" t="s">
+        <v>213</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I65" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="1">
         <v>4.5678901E7</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>211</v>
+      <c r="B66" s="7" t="s">
+        <v>216</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>212</v>
+        <v>217</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I66" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="1">
         <v>5.6789012E7</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>213</v>
+      <c r="B67" s="7" t="s">
+        <v>218</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>215</v>
+        <v>220</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I67" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="1">
         <v>6.7890123E7</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>216</v>
+      <c r="B68" s="7" t="s">
+        <v>221</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>218</v>
+        <v>223</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I68" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="1">
         <v>7.8901234E7</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>219</v>
+      <c r="B69" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>222</v>
+        <v>227</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I69" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="1">
         <v>8.9012345E7</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>223</v>
+      <c r="B70" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>226</v>
+        <v>231</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I70" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="1">
         <v>9.0123456E7</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>227</v>
+      <c r="B71" s="7" t="s">
+        <v>232</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>228</v>
+        <v>233</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I71" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="1">
         <v>1.2345677E7</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>229</v>
+      <c r="B72" s="7" t="s">
+        <v>234</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>231</v>
+        <v>236</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I72" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="1">
         <v>2.1487654E7</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="D73" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>235</v>
+      <c r="B73" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>240</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>236</v>
+        <v>241</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I73" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="1">
         <v>2.0928175E7</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>11</v>
+      <c r="B74" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>240</v>
+        <v>245</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I74" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="1">
         <v>2.1765423E7</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>242</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>243</v>
+      <c r="B75" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>248</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>244</v>
+        <v>249</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I75" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="1">
         <v>2.0387129E7</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>246</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>248</v>
+      <c r="B76" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>253</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>249</v>
+        <v>254</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I76" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="1">
         <v>2.1123456E7</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>252</v>
+      <c r="B77" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>257</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>253</v>
+        <v>258</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I77" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="1">
         <v>2.156789E7</v>
       </c>
-      <c r="B78" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>255</v>
+      <c r="B78" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>260</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>256</v>
+        <v>261</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I78" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="1">
         <v>2.1987654E7</v>
       </c>
-      <c r="B79" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>260</v>
+      <c r="B79" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>265</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>261</v>
+        <v>266</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I79" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="1">
         <v>2.0654321E7</v>
       </c>
-      <c r="B80" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>265</v>
+      <c r="B80" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>270</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>266</v>
+        <v>271</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I80" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="1">
         <v>2.1345678E7</v>
       </c>
-      <c r="B81" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="D81" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>270</v>
+      <c r="B81" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>275</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>271</v>
+        <v>276</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I81" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="1">
         <v>1.1111222E7</v>
       </c>
-      <c r="B82" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>130</v>
+      <c r="B82" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>273</v>
+        <v>278</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I82" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="1">
         <v>2.2223333E7</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="7" t="s">
-        <v>243</v>
+      <c r="B83" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>248</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>275</v>
+        <v>280</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I83" s="5">
+        <v>2021.0</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="1">
         <v>3.3334444E7</v>
       </c>
-      <c r="B84" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="E84" s="7" t="s">
-        <v>278</v>
+      <c r="B84" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>283</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>279</v>
+        <v>284</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I84" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="1">
         <v>4.4445555E7</v>
       </c>
-      <c r="B85" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E85" s="7" t="s">
+      <c r="B85" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="H85" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F85" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>282</v>
+      <c r="I85" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="1">
         <v>5.5556666E7</v>
       </c>
-      <c r="B86" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>141</v>
+      <c r="B86" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>285</v>
+        <v>290</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I86" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="1">
         <v>6.6667777E7</v>
       </c>
-      <c r="B87" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D87" s="7" t="s">
+      <c r="B87" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E87" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E87" s="7" t="s">
-        <v>23</v>
-      </c>
       <c r="F87" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>287</v>
+        <v>292</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I87" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="1">
         <v>7.7778888E7</v>
       </c>
-      <c r="B88" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>243</v>
+      <c r="B88" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>248</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>290</v>
+        <v>295</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I88" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="1">
         <v>8.8889999E7</v>
       </c>
-      <c r="B89" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="D89" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>225</v>
+      <c r="B89" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>293</v>
+        <v>298</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I89" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="1">
         <v>9.999E7</v>
       </c>
-      <c r="B90" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="D90" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>137</v>
+      <c r="B90" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>142</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>297</v>
+        <v>302</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I90" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="1">
         <v>1.1112222E7</v>
       </c>
-      <c r="B91" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>209</v>
+      <c r="B91" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>300</v>
+        <v>305</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I91" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="1">
         <v>2.2223333E7</v>
       </c>
-      <c r="B92" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="E92" s="7" t="s">
-        <v>130</v>
+      <c r="B92" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>303</v>
+        <v>308</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I92" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="1">
         <v>3.3334444E7</v>
       </c>
-      <c r="B93" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D93" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E93" s="7" t="s">
-        <v>141</v>
+      <c r="B93" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>164</v>
+        <v>169</v>
+      </c>
+      <c r="H93" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I93" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="1">
         <v>1.3047963E7</v>
       </c>
-      <c r="B94" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D94" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="E94" s="7" t="s">
-        <v>130</v>
+      <c r="B94" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="C94" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>135</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>307</v>
+        <v>312</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I94" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="1">
         <v>2.1479513E7</v>
       </c>
-      <c r="B95" s="5" t="s">
-        <v>308</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>54</v>
+      <c r="B95" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>312</v>
+        <v>317</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I95" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="1">
         <v>1.570238E7</v>
       </c>
-      <c r="B96" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>314</v>
-      </c>
-      <c r="D96" s="7" t="s">
-        <v>315</v>
-      </c>
-      <c r="E96" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>54</v>
+      <c r="B96" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="C96" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>316</v>
+        <v>321</v>
+      </c>
+      <c r="H96" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I96" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="1">
         <v>1.9073284E7</v>
       </c>
-      <c r="B97" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>141</v>
+      <c r="B97" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>320</v>
+        <v>325</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I97" s="5">
+        <v>2022.0</v>
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="1">
         <v>1.6134702E7</v>
       </c>
-      <c r="B98" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="D98" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="E98" s="7" t="s">
+      <c r="B98" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C98" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H98" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F98" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>324</v>
+      <c r="I98" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="1">
         <v>1.7829051E7</v>
       </c>
-      <c r="B99" s="5" t="s">
-        <v>325</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D99" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>85</v>
+      <c r="B99" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>327</v>
+        <v>332</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I99" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="1">
         <v>2.0571439E7</v>
       </c>
-      <c r="B100" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="C100" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="E100" s="7" t="s">
-        <v>225</v>
+      <c r="B100" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>330</v>
+        <v>335</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I100" s="5">
+        <v>2023.0</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1"/>

</xml_diff>